<commit_message>
Fix Ray's feedback on cable counts
</commit_message>
<xml_diff>
--- a/events/metropolist/2023-02-25/Metropolist.xlsx
+++ b/events/metropolist/2023-02-25/Metropolist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Power</t>
   </si>
@@ -46,16 +46,16 @@
     <t xml:space="preserve">Circuts</t>
   </si>
   <si>
-    <t xml:space="preserve">4'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32'</t>
+    <t xml:space="preserve">5’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50’</t>
   </si>
   <si>
     <t xml:space="preserve">3/5 Pin Converters</t>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">Edison → True1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edison → IEC</t>
   </si>
   <si>
     <t xml:space="preserve">24’ Extension</t>
@@ -386,10 +383,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1048576"/>
+  <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -402,7 +399,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,12 +425,11 @@
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -486,14 +481,11 @@
       <c r="Q2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -513,16 +505,15 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
@@ -533,33 +524,34 @@
       <c r="H4" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="J4" s="12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="O4" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="P4" s="8" t="n">
         <v>4</v>
       </c>
       <c r="Q4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="R4" s="8" t="n">
-        <v>4</v>
-      </c>
+      <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="10" t="n">
         <v>2</v>
@@ -588,16 +580,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>1</v>
@@ -626,16 +617,15 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>3</v>
@@ -655,23 +645,20 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="12" t="n">
-        <v>12</v>
-      </c>
+      <c r="K7" s="12"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8" t="n">
+      <c r="N7" s="8" t="n">
         <v>12</v>
       </c>
+      <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
@@ -686,7 +673,7 @@
         <v>27.08</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -699,14 +686,13 @@
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
+      <c r="R8" s="13"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
       <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
@@ -726,18 +712,17 @@
       <c r="O9" s="18"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="R9" s="9"/>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
+      <c r="W9" s="13"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -752,19 +737,18 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="O10" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="P10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="R10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
@@ -784,12 +768,11 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
+      <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
@@ -806,15 +789,14 @@
       <c r="L12" s="8"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
+      <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
+      <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="2"/>
+      <c r="V12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
@@ -831,15 +813,14 @@
       <c r="L13" s="8"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
+      <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="R13" s="2"/>
       <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
+      <c r="T13" s="10"/>
       <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="2"/>
+      <c r="V13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
@@ -859,14 +840,13 @@
       <c r="O14" s="18"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
+      <c r="W14" s="13"/>
       <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
@@ -883,17 +863,16 @@
       <c r="L15" s="18"/>
       <c r="M15" s="8"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
+      <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="W15" s="13"/>
       <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
@@ -910,15 +889,14 @@
       <c r="L16" s="8"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
+      <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
+      <c r="T16" s="10"/>
       <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="2"/>
+      <c r="V16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
@@ -938,12 +916,11 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
+      <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
@@ -963,14 +940,13 @@
       <c r="O18" s="18"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
+      <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
+      <c r="W18" s="13"/>
       <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
@@ -990,14 +966,13 @@
       <c r="O19" s="18"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
+      <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
+      <c r="W19" s="13"/>
       <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
@@ -1014,17 +989,16 @@
       <c r="L20" s="8"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
+      <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
+      <c r="W20" s="13"/>
       <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
@@ -1044,14 +1018,13 @@
       <c r="O21" s="18"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
+      <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
+      <c r="W21" s="13"/>
       <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
@@ -1069,16 +1042,15 @@
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
+      <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
+      <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
+      <c r="W22" s="13"/>
       <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
@@ -1096,14 +1068,13 @@
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
+      <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
@@ -1121,14 +1092,13 @@
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
+      <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
@@ -1146,14 +1116,13 @@
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
+      <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
+      <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
@@ -1170,10 +1139,9 @@
       <c r="L26" s="22"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
@@ -1191,14 +1159,13 @@
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
+      <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
+      <c r="R27" s="10"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
@@ -1218,12 +1185,11 @@
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
+      <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
@@ -1241,14 +1207,13 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
+      <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
+      <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
-      <c r="W29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
@@ -1268,12 +1233,11 @@
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
+      <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
@@ -1290,15 +1254,14 @@
       <c r="L31" s="8"/>
       <c r="M31" s="19"/>
       <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="O31" s="19"/>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
+      <c r="R31" s="2"/>
       <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
@@ -1318,12 +1281,11 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
+      <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
@@ -1343,12 +1305,11 @@
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
+      <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
@@ -1368,12 +1329,11 @@
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
+      <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
@@ -1393,12 +1353,11 @@
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
+      <c r="R35" s="2"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
@@ -1418,12 +1377,11 @@
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+      <c r="R36" s="2"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
@@ -1440,15 +1398,14 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
+      <c r="R37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
@@ -1468,12 +1425,11 @@
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
+      <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
@@ -1496,12 +1452,11 @@
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
+      <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
@@ -1509,7 +1464,7 @@
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" s="11" t="n">
         <v>2</v>
@@ -1524,15 +1479,15 @@
       </c>
       <c r="I40" s="12" t="n">
         <f aca="false">SUM(I3:I38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40" s="12" t="n">
         <f aca="false">SUM(J3:J38)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K40" s="12" t="n">
         <f aca="false">SUM(K3:K39)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L40" s="8"/>
       <c r="M40" s="19" t="n">
@@ -1541,11 +1496,11 @@
       </c>
       <c r="N40" s="19" t="n">
         <f aca="false">SUM(N3:N39)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O40" s="19" t="n">
         <f aca="false">SUM(O3:O39)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P40" s="19" t="n">
         <f aca="false">SUM(P3:P39)</f>
@@ -1553,17 +1508,13 @@
       </c>
       <c r="Q40" s="19" t="n">
         <f aca="false">SUM(Q3:Q39)</f>
-        <v>5</v>
-      </c>
-      <c r="R40" s="19" t="n">
-        <f aca="false">SUM(R3:R39)</f>
         <v>4</v>
       </c>
+      <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
@@ -1571,7 +1522,7 @@
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="11" t="n">
         <v>0</v>
@@ -1592,14 +1543,13 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F42" s="11" t="n">
         <v>2</v>
@@ -1626,7 +1576,6 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="10"/>
@@ -1634,7 +1583,7 @@
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G40*1.05)</f>
@@ -1646,15 +1595,15 @@
       </c>
       <c r="I44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I40*1.05)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(J40*1.05)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K44" s="10" t="n">
         <f aca="false">ROUND(K40*1.05,0)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="10" t="n">
@@ -1663,11 +1612,11 @@
       </c>
       <c r="N44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(N40*1.05)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="O44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(O40*1.05)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="P44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(P40*1.05)</f>
@@ -1675,17 +1624,13 @@
       </c>
       <c r="Q44" s="10" t="n">
         <f aca="false">_xlfn.CEILING.MATH(Q40*1.05)</f>
-        <v>6</v>
-      </c>
-      <c r="R44" s="10" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(R40*1.05)</f>
         <v>5</v>
       </c>
+      <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="10"/>
@@ -1769,7 +1714,7 @@
   <mergeCells count="3">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Fixed incorrect power info
</commit_message>
<xml_diff>
--- a/events/metropolist/2023-02-25/Metropolist.xlsx
+++ b/events/metropolist/2023-02-25/Metropolist.xlsx
@@ -88,10 +88,10 @@
     <t xml:space="preserve">Vizi Beam 12RX</t>
   </si>
   <si>
-    <t xml:space="preserve">12P Hex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x2 15A</t>
+    <t xml:space="preserve">12P Hex IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x4 15A</t>
   </si>
   <si>
     <t xml:space="preserve">Tech Table</t>
@@ -386,7 +386,7 @@
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,7 +397,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="3.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.34"/>
   </cols>
   <sheetData>
@@ -594,11 +594,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>0.13</v>
+        <v>3.2</v>
       </c>
       <c r="D6" s="11" t="n">
         <f aca="false">C6*B6</f>
-        <v>0.13</v>
+        <v>3.2</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -631,11 +631,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="11" t="n">
-        <v>0.68</v>
+        <v>1.25</v>
       </c>
       <c r="D7" s="11" t="n">
         <f aca="false">C7*B7</f>
-        <v>2.04</v>
+        <v>3.75</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -666,11 +666,11 @@
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="n">
         <f aca="false">SUM(D5:D7)</f>
-        <v>6.77</v>
+        <v>11.55</v>
       </c>
       <c r="E8" s="15" t="n">
         <f aca="false">D8*4</f>
-        <v>27.08</v>
+        <v>46.2</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>23</v>
@@ -1438,7 +1438,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="11" t="n">
         <f aca="false">SUM(E4:E38)</f>
-        <v>27.08</v>
+        <v>46.2</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="12"/>
@@ -1467,7 +1467,7 @@
         <v>25</v>
       </c>
       <c r="F40" s="11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G40" s="12" t="n">
         <f aca="false">SUM(G3:G38)</f>
@@ -1552,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="F42" s="11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>